<commit_message>
Refactoring of SheetDSVConverter and SheetODSCOnverter
</commit_message>
<xml_diff>
--- a/test/sheet/fixtures/simple.xlsx
+++ b/test/sheet/fixtures/simple.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,13 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t xml:space="preserve">field1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">field2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">a</t>
   </si>
@@ -49,6 +43,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -134,46 +129,38 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>2</v>
+      <c r="A2" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
+      <c r="A3" s="0" t="s">
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="0" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>